<commit_message>
Allow G rated to get heat pumps
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_Retrofit-Ctrl.xlsx
+++ b/SuppXLS/Scen_B_RSD_Retrofit-Ctrl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BBF079-DD13-46C1-9F0F-AC19A58436C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27D6791-952E-400E-BA8B-89CBCE5632CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
@@ -573,11 +573,18 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -775,7 +782,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1133,228 +1140,253 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="11" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="11" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="11" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="11" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="11" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="11" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2491,12 +2523,12 @@
       <c r="Z15" s="15"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="18"/>
@@ -2580,11 +2612,11 @@
       <c r="A19" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -2612,11 +2644,11 @@
       <c r="A20" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
       <c r="G20" s="24"/>
@@ -2704,11 +2736,11 @@
       <c r="A23" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
@@ -2734,11 +2766,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -2794,11 +2826,11 @@
       <c r="A26" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -2824,11 +2856,11 @@
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -2916,11 +2948,11 @@
       <c r="A30" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
       <c r="G30" s="15"/>
@@ -2948,11 +2980,11 @@
       <c r="A31" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
       <c r="G31" s="15"/>
@@ -5678,8 +5710,8 @@
   </sheetPr>
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5727,31 +5759,31 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="69" t="s">
+      <c r="E7" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="69">
+      <c r="F7" s="48">
         <v>2018</v>
       </c>
-      <c r="G7" s="69">
+      <c r="G7" s="48">
         <v>2030</v>
       </c>
-      <c r="H7" s="69">
+      <c r="H7" s="48">
         <v>2070</v>
       </c>
-      <c r="I7" s="69" t="s">
+      <c r="I7" s="48" t="s">
         <v>4</v>
       </c>
       <c r="K7" s="3" t="s">
@@ -5776,15 +5808,15 @@
       <c r="E8" s="2">
         <v>1</v>
       </c>
-      <c r="F8" s="72">
+      <c r="F8" s="51">
         <f>($E$43*F$29)/1000</f>
         <v>3.042234442534121</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="51">
         <f>(E43*G$28)/1000</f>
         <v>11.408379159502955</v>
       </c>
-      <c r="H8" s="72">
+      <c r="H8" s="51">
         <f>(H43*H$27)/1000</f>
         <v>12.041696314577493</v>
       </c>
@@ -5813,15 +5845,15 @@
       <c r="E9" s="2">
         <v>1</v>
       </c>
-      <c r="F9" s="72">
+      <c r="F9" s="51">
         <f>($E$42*F$29)/1000</f>
         <v>2.4662346453768067</v>
       </c>
-      <c r="G9" s="72">
+      <c r="G9" s="51">
         <f>(E42*G$28)/1000</f>
         <v>9.2483799201630248</v>
       </c>
-      <c r="H9" s="72">
+      <c r="H9" s="51">
         <f>(H42*H$27)/1000</f>
         <v>9.7617883174643403</v>
       </c>
@@ -5850,15 +5882,15 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="51">
         <f>($E$41*F$29)/1000</f>
         <v>5.153575294552267</v>
       </c>
-      <c r="G10" s="72">
+      <c r="G10" s="51">
         <f>(E41*G$28)/1000</f>
         <v>19.325907354571001</v>
       </c>
-      <c r="H10" s="72">
+      <c r="H10" s="51">
         <f>(H41*H$27)/1000</f>
         <v>20.398752891514416</v>
       </c>
@@ -5887,15 +5919,15 @@
       <c r="E11" s="2">
         <v>1</v>
       </c>
-      <c r="F11" s="72">
+      <c r="F11" s="51">
         <f>($E$40*F$29)/1000</f>
         <v>8.7478683298212321</v>
       </c>
-      <c r="G11" s="72">
+      <c r="G11" s="51">
         <f>(E40*G$28)/1000</f>
         <v>32.804506236829617</v>
       </c>
-      <c r="H11" s="72">
+      <c r="H11" s="51">
         <f>(H40*H$27)/1000</f>
         <v>34.62559372639015</v>
       </c>
@@ -5924,15 +5956,15 @@
       <c r="E12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" s="72">
+      <c r="F12" s="51">
         <f>($E$39*F$29)/1000</f>
         <v>11.78096068728674</v>
       </c>
-      <c r="G12" s="72">
+      <c r="G12" s="51">
         <f>(E39*G$28)/1000</f>
         <v>44.178602577325279</v>
       </c>
-      <c r="H12" s="72">
+      <c r="H12" s="51">
         <f>(H39*H$27)/1000</f>
         <v>46.6311040684012</v>
       </c>
@@ -5944,36 +5976,36 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="70" t="str">
+      <c r="A13" s="49" t="str">
         <f>"UC_RSD_RTFT_"&amp;RIGHT(C13,6)</f>
         <v>UC_RSD_RTFT_Apt_B3</v>
       </c>
-      <c r="B13" s="70" t="str">
+      <c r="B13" s="49" t="str">
         <f>"Maximum number of deep retrofits from Apartment_" &amp;RIGHT(C13,2)</f>
         <v>Maximum number of deep retrofits from Apartment_B3</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="70">
+      <c r="E13" s="49">
         <v>1</v>
       </c>
-      <c r="F13" s="73">
+      <c r="F13" s="52">
         <f>($E$38*F$29)/1000</f>
         <v>3.9848960750111653</v>
       </c>
-      <c r="G13" s="73">
+      <c r="G13" s="52">
         <f>(E38*G$28)/1000</f>
         <v>14.943360281291868</v>
       </c>
-      <c r="H13" s="73">
+      <c r="H13" s="52">
         <f>(H38*H$27)/1000</f>
         <v>15.772916021707317</v>
       </c>
-      <c r="I13" s="70">
+      <c r="I13" s="49">
         <v>5</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -5981,36 +6013,36 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="71" t="str">
+      <c r="A14" s="50" t="str">
         <f>"UC_RSD_RTFT_"&amp;RIGHT(C14,5)</f>
         <v>UC_RSD_RTFT_Att_G</v>
       </c>
-      <c r="B14" s="71" t="str">
+      <c r="B14" s="50" t="str">
         <f>"Maximum number of deep retrofits from Attached_" &amp;RIGHT(C14,1)</f>
         <v>Maximum number of deep retrofits from Attached_G</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="71">
+      <c r="E14" s="50">
         <v>1</v>
       </c>
-      <c r="F14" s="74">
+      <c r="F14" s="53">
         <f>($C$43*F$29)/1000</f>
         <v>10.541334878817622</v>
       </c>
-      <c r="G14" s="74">
+      <c r="G14" s="53">
         <f>(C43*G$28)/1000</f>
         <v>39.530005795566083</v>
       </c>
-      <c r="H14" s="74">
+      <c r="H14" s="53">
         <f>(F43*H$27)/1000</f>
         <v>41.724448183963943</v>
       </c>
-      <c r="I14" s="71">
+      <c r="I14" s="50">
         <v>5</v>
       </c>
       <c r="K14" s="2" t="s">
@@ -6035,15 +6067,15 @@
       <c r="E15" s="13">
         <v>1</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="54">
         <f>($C$42*F$29)/1000</f>
         <v>10.024761205464234</v>
       </c>
-      <c r="G15" s="75">
+      <c r="G15" s="54">
         <f>(C42*G$28)/1000</f>
         <v>37.592854520490874</v>
       </c>
-      <c r="H15" s="75">
+      <c r="H15" s="54">
         <f>(F42*H$27)/1000</f>
         <v>39.679759184438389</v>
       </c>
@@ -6072,15 +6104,15 @@
       <c r="E16" s="13">
         <v>1</v>
       </c>
-      <c r="F16" s="75">
+      <c r="F16" s="54">
         <f>($C$41*F$29)/1000</f>
         <v>20.283779192369344</v>
       </c>
-      <c r="G16" s="75">
+      <c r="G16" s="54">
         <f>(C41*G$28)/1000</f>
         <v>76.064171971385051</v>
       </c>
-      <c r="H16" s="75">
+      <c r="H16" s="54">
         <f>(F41*H$27)/1000</f>
         <v>80.286747704756522</v>
       </c>
@@ -6109,15 +6141,15 @@
       <c r="E17" s="13">
         <v>1</v>
       </c>
-      <c r="F17" s="75">
+      <c r="F17" s="54">
         <f>($C$40*F$29)/1000</f>
         <v>37.525404475322098</v>
       </c>
-      <c r="G17" s="75">
+      <c r="G17" s="54">
         <f>(C40*G$28)/1000</f>
         <v>140.72026678245786</v>
       </c>
-      <c r="H17" s="75">
+      <c r="H17" s="54">
         <f>(F40*H$27)/1000</f>
         <v>148.53211785910801</v>
       </c>
@@ -6146,15 +6178,15 @@
       <c r="E18" s="13">
         <v>1</v>
       </c>
-      <c r="F18" s="75">
+      <c r="F18" s="54">
         <f>($C$39*F$29)/1000</f>
         <v>56.430305495129602</v>
       </c>
-      <c r="G18" s="75">
+      <c r="G18" s="54">
         <f>(C39*G$28)/1000</f>
         <v>211.61364560673599</v>
       </c>
-      <c r="H18" s="75">
+      <c r="H18" s="54">
         <f>(F39*H$27)/1000</f>
         <v>223.3610244531846</v>
       </c>
@@ -6166,36 +6198,36 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="70" t="str">
+      <c r="A19" s="49" t="str">
         <f>"UC_RSD_RTFT_"&amp;RIGHT(C19,6)</f>
         <v>UC_RSD_RTFT_Att_B3</v>
       </c>
-      <c r="B19" s="70" t="str">
+      <c r="B19" s="49" t="str">
         <f>"Maximum number of deep retrofits from Attached_" &amp;RIGHT(C19,2)</f>
         <v>Maximum number of deep retrofits from Attached_B3</v>
       </c>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="70" t="s">
+      <c r="D19" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="70">
+      <c r="E19" s="49">
         <v>1</v>
       </c>
-      <c r="F19" s="73">
+      <c r="F19" s="52">
         <f>($C$38*F$29)/1000</f>
         <v>9.9537699371858963</v>
       </c>
-      <c r="G19" s="73">
+      <c r="G19" s="52">
         <f>(C38*G$28)/1000</f>
         <v>37.326637264447108</v>
       </c>
-      <c r="H19" s="73">
+      <c r="H19" s="52">
         <f>(F38*H$27)/1000</f>
         <v>39.398763321120782</v>
       </c>
-      <c r="I19" s="70">
+      <c r="I19" s="49">
         <v>5</v>
       </c>
       <c r="K19" s="2" t="s">
@@ -6203,36 +6235,36 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="71" t="str">
+      <c r="A20" s="50" t="str">
         <f>"UC_RSD_RTFT_"&amp;RIGHT(C20,5)</f>
         <v>UC_RSD_RTFT_Det_G</v>
       </c>
-      <c r="B20" s="71" t="str">
+      <c r="B20" s="50" t="str">
         <f>"Maximum number of deep retrofits from Detached_" &amp;RIGHT(C20,1)</f>
         <v>Maximum number of deep retrofits from Detached_G</v>
       </c>
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="71">
+      <c r="E20" s="50">
         <v>1</v>
       </c>
-      <c r="F20" s="74">
+      <c r="F20" s="53">
         <f>($D$43*F$29)/1000</f>
         <v>15.687106688620966</v>
       </c>
-      <c r="G20" s="74">
+      <c r="G20" s="53">
         <f>(D43*G$28)/1000</f>
         <v>58.826650082328619</v>
       </c>
-      <c r="H20" s="74">
+      <c r="H20" s="53">
         <f>(G43*H$27)/1000</f>
         <v>62.092313517232284</v>
       </c>
-      <c r="I20" s="71">
+      <c r="I20" s="50">
         <v>5</v>
       </c>
       <c r="K20" s="13" t="s">
@@ -6257,15 +6289,15 @@
       <c r="E21" s="13">
         <v>1</v>
       </c>
-      <c r="F21" s="75">
+      <c r="F21" s="54">
         <f>($D$42*F$29)/1000</f>
         <v>8.6482011525934226</v>
       </c>
-      <c r="G21" s="75">
+      <c r="G21" s="54">
         <f>(D42*G$28)/1000</f>
         <v>32.43075432222534</v>
       </c>
-      <c r="H21" s="75">
+      <c r="H21" s="54">
         <f>(G42*H$27)/1000</f>
         <v>34.23109359716647</v>
       </c>
@@ -6294,15 +6326,15 @@
       <c r="E22" s="13">
         <v>1</v>
       </c>
-      <c r="F22" s="75">
+      <c r="F22" s="54">
         <f>($D$41*F$29)/1000</f>
         <v>16.279339597911104</v>
       </c>
-      <c r="G22" s="75">
+      <c r="G22" s="54">
         <f>(D41*G$28)/1000</f>
         <v>61.047523492166633</v>
       </c>
-      <c r="H22" s="75">
+      <c r="H22" s="54">
         <f>(G41*H$27)/1000</f>
         <v>64.436475012961779</v>
       </c>
@@ -6331,15 +6363,15 @@
       <c r="E23" s="13">
         <v>1</v>
       </c>
-      <c r="F23" s="75">
+      <c r="F23" s="54">
         <f>($D$40*F$29)/1000</f>
         <v>33.333558282558243</v>
       </c>
-      <c r="G23" s="75">
+      <c r="G23" s="54">
         <f>(D40*G$28)/1000</f>
         <v>125.00084355959343</v>
       </c>
-      <c r="H23" s="75">
+      <c r="H23" s="54">
         <f>(G40*H$27)/1000</f>
         <v>131.94005705506501</v>
       </c>
@@ -6368,15 +6400,15 @@
       <c r="E24" s="13">
         <v>1</v>
       </c>
-      <c r="F24" s="75">
+      <c r="F24" s="54">
         <f>($D$39*F$29)/1000</f>
         <v>50.263786722748698</v>
       </c>
-      <c r="G24" s="75">
+      <c r="G24" s="54">
         <f>(D39*G$28)/1000</f>
         <v>188.48920021030762</v>
       </c>
-      <c r="H24" s="75">
+      <c r="H24" s="54">
         <f>(G39*H$27)/1000</f>
         <v>198.9528640113158</v>
       </c>
@@ -6388,36 +6420,36 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="70" t="str">
+      <c r="A25" s="49" t="str">
         <f>"UC_RSD_RTFT_"&amp;RIGHT(C25,6)</f>
         <v>UC_RSD_RTFT_Det_B3</v>
       </c>
-      <c r="B25" s="70" t="str">
+      <c r="B25" s="49" t="str">
         <f>"Maximum number of deep retrofits from Detached_" &amp;RIGHT(C25,2)</f>
         <v>Maximum number of deep retrofits from Detached_B3</v>
       </c>
-      <c r="C25" s="70" t="s">
+      <c r="C25" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="D25" s="70" t="s">
+      <c r="D25" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="70">
+      <c r="E25" s="49">
         <v>1</v>
       </c>
-      <c r="F25" s="73">
+      <c r="F25" s="52">
         <f>($D$38*F$29)/1000</f>
         <v>10.693242008796334</v>
       </c>
-      <c r="G25" s="73">
+      <c r="G25" s="52">
         <f>(D38*G$28)/1000</f>
         <v>40.099657532986257</v>
       </c>
-      <c r="H25" s="73">
+      <c r="H25" s="52">
         <f>(G38*H$27)/1000</f>
         <v>42.32572318816743</v>
       </c>
-      <c r="I25" s="70">
+      <c r="I25" s="49">
         <v>5</v>
       </c>
       <c r="J25" s="13"/>
@@ -6427,32 +6459,32 @@
     </row>
     <row r="26" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="38"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
       <c r="G27" s="2"/>
       <c r="H27" s="30">
         <v>0.95</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="39" t="s">
+      <c r="C28" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="40"/>
-      <c r="E28" s="41"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="72"/>
       <c r="G28" s="30">
         <v>0.75</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="44"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="75"/>
       <c r="F29" s="31">
         <v>0.2</v>
       </c>
@@ -6462,306 +6494,306 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
-      <c r="H32" s="53"/>
-      <c r="K32" s="54" t="s">
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="60"/>
+      <c r="K32" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="L32" s="55"/>
-      <c r="M32" s="56"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="66"/>
     </row>
     <row r="33" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
-      <c r="C33" s="51">
+      <c r="C33" s="58">
         <v>2018</v>
       </c>
-      <c r="D33" s="52"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="36">
+      <c r="D33" s="59"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="61">
         <v>2070</v>
       </c>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
-      <c r="K33" s="57">
+      <c r="G33" s="62"/>
+      <c r="H33" s="63"/>
+      <c r="K33" s="67">
         <v>0.83330000000000004</v>
       </c>
-      <c r="L33" s="58"/>
-      <c r="M33" s="59"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="69"/>
     </row>
     <row r="34" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="67" t="s">
+      <c r="C34" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="67" t="s">
+      <c r="D34" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="67" t="s">
+      <c r="E34" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="67" t="s">
+      <c r="F34" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="G34" s="67" t="s">
+      <c r="G34" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="H34" s="68" t="s">
+      <c r="H34" s="47" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="35" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="46">
-        <v>15472.073727176739</v>
-      </c>
-      <c r="D35" s="46">
-        <v>20378.706337556119</v>
-      </c>
-      <c r="E35" s="46">
-        <v>9418.8988568067343</v>
-      </c>
-      <c r="F35" s="46">
+      <c r="C35" s="76">
+        <v>37224.073727176743</v>
+      </c>
+      <c r="D35" s="76">
+        <v>31387.706337556119</v>
+      </c>
+      <c r="E35" s="76">
+        <v>14540.898856806734</v>
+      </c>
+      <c r="F35" s="34">
         <f>C35*$K$33</f>
-        <v>12892.879036856377</v>
-      </c>
-      <c r="G35" s="46">
+        <v>31018.820636856381</v>
+      </c>
+      <c r="G35" s="34">
         <f>D35*$K$33</f>
-        <v>16981.575991085516</v>
-      </c>
-      <c r="H35" s="60">
+        <v>26155.375691085515</v>
+      </c>
+      <c r="H35" s="39">
         <f>E35*$K$33</f>
-        <v>7848.7684173770522</v>
+        <v>12116.931017377052</v>
       </c>
     </row>
     <row r="36" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="48">
+      <c r="C36" s="77">
         <v>9537.7783975583752</v>
       </c>
-      <c r="D36" s="48">
+      <c r="D36" s="77">
         <v>9433.9012004747347</v>
       </c>
-      <c r="E36" s="48">
+      <c r="E36" s="77">
         <v>7459.2913438514906</v>
       </c>
-      <c r="F36" s="48">
+      <c r="F36" s="36">
         <f t="shared" ref="F36:F43" si="4">C36*$K$33</f>
         <v>7947.8307386853949</v>
       </c>
-      <c r="G36" s="48">
+      <c r="G36" s="36">
         <f t="shared" ref="G36:G43" si="5">D36*$K$33</f>
         <v>7861.269870355597</v>
       </c>
-      <c r="H36" s="61">
+      <c r="H36" s="40">
         <f t="shared" ref="H36:H43" si="6">E36*$K$33</f>
         <v>6215.8274768314477</v>
       </c>
     </row>
     <row r="37" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="50">
+      <c r="C37" s="78">
         <v>17545.09295382088</v>
       </c>
-      <c r="D37" s="50">
+      <c r="D37" s="78">
         <v>20090.949195825138</v>
       </c>
-      <c r="E37" s="50">
+      <c r="E37" s="78">
         <v>14041.847426430093</v>
       </c>
-      <c r="F37" s="50">
+      <c r="F37" s="38">
         <f t="shared" si="4"/>
         <v>14620.32595841894</v>
       </c>
-      <c r="G37" s="50">
+      <c r="G37" s="38">
         <f t="shared" si="5"/>
         <v>16741.787964881089</v>
       </c>
-      <c r="H37" s="62">
+      <c r="H37" s="41">
         <f t="shared" si="6"/>
         <v>11701.071460444196</v>
       </c>
     </row>
     <row r="38" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="48">
+      <c r="C38" s="77">
         <v>49768.849685929476</v>
       </c>
-      <c r="D38" s="48">
+      <c r="D38" s="77">
         <v>53466.210043981671</v>
       </c>
-      <c r="E38" s="48">
+      <c r="E38" s="77">
         <v>19924.480375055824</v>
       </c>
-      <c r="F38" s="48">
+      <c r="F38" s="36">
         <f t="shared" si="4"/>
         <v>41472.382443285031</v>
       </c>
-      <c r="G38" s="48">
+      <c r="G38" s="36">
         <f t="shared" si="5"/>
         <v>44553.392829649929</v>
       </c>
-      <c r="H38" s="61">
+      <c r="H38" s="40">
         <f t="shared" si="6"/>
         <v>16603.069496534019</v>
       </c>
     </row>
     <row r="39" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B39" s="49" t="s">
+      <c r="B39" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="50">
+      <c r="C39" s="78">
         <v>282151.52747564798</v>
       </c>
-      <c r="D39" s="50">
+      <c r="D39" s="78">
         <v>251318.93361374349</v>
       </c>
-      <c r="E39" s="50">
+      <c r="E39" s="78">
         <v>58904.8034364337</v>
       </c>
-      <c r="F39" s="50">
+      <c r="F39" s="38">
         <f t="shared" si="4"/>
         <v>235116.86784545748</v>
       </c>
-      <c r="G39" s="50">
+      <c r="G39" s="38">
         <f t="shared" si="5"/>
         <v>209424.06738033245</v>
       </c>
-      <c r="H39" s="62">
+      <c r="H39" s="41">
         <f t="shared" si="6"/>
         <v>49085.372703580208</v>
       </c>
     </row>
     <row r="40" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="48">
+      <c r="C40" s="77">
         <v>187627.02237661046</v>
       </c>
-      <c r="D40" s="48">
+      <c r="D40" s="77">
         <v>166667.79141279124</v>
       </c>
-      <c r="E40" s="48">
+      <c r="E40" s="77">
         <v>43739.341649106158</v>
       </c>
-      <c r="F40" s="48">
+      <c r="F40" s="36">
         <f t="shared" si="4"/>
         <v>156349.5977464295</v>
       </c>
-      <c r="G40" s="48">
+      <c r="G40" s="36">
         <f t="shared" si="5"/>
         <v>138884.27058427894</v>
       </c>
-      <c r="H40" s="61">
+      <c r="H40" s="40">
         <f t="shared" si="6"/>
         <v>36447.99339620016</v>
       </c>
     </row>
     <row r="41" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="50">
+      <c r="C41" s="78">
         <v>101418.89596184672</v>
       </c>
-      <c r="D41" s="50">
+      <c r="D41" s="78">
         <v>81396.697989555512</v>
       </c>
-      <c r="E41" s="50">
+      <c r="E41" s="78">
         <v>25767.876472761334</v>
       </c>
-      <c r="F41" s="50">
+      <c r="F41" s="38">
         <f t="shared" si="4"/>
         <v>84512.366005006872</v>
       </c>
-      <c r="G41" s="50">
+      <c r="G41" s="38">
         <f t="shared" si="5"/>
         <v>67827.868434696618</v>
       </c>
-      <c r="H41" s="62">
+      <c r="H41" s="41">
         <f t="shared" si="6"/>
         <v>21472.371464752021</v>
       </c>
     </row>
     <row r="42" spans="2:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B42" s="47" t="s">
+      <c r="B42" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="48">
+      <c r="C42" s="77">
         <v>50123.806027321167</v>
       </c>
-      <c r="D42" s="48">
+      <c r="D42" s="77">
         <v>43241.005762967114</v>
       </c>
-      <c r="E42" s="48">
+      <c r="E42" s="77">
         <v>12331.173226884033</v>
       </c>
-      <c r="F42" s="48">
+      <c r="F42" s="36">
         <f t="shared" si="4"/>
         <v>41768.167562566727</v>
       </c>
-      <c r="G42" s="48">
+      <c r="G42" s="36">
         <f t="shared" si="5"/>
         <v>36032.730102280497</v>
       </c>
-      <c r="H42" s="61">
+      <c r="H42" s="40">
         <f t="shared" si="6"/>
         <v>10275.566649962466</v>
       </c>
     </row>
     <row r="43" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="63" t="s">
+      <c r="B43" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="64">
+      <c r="C43" s="79">
         <v>52706.674394088106</v>
       </c>
-      <c r="D43" s="64">
+      <c r="D43" s="79">
         <v>78435.533443104825</v>
       </c>
-      <c r="E43" s="64">
+      <c r="E43" s="79">
         <v>15211.172212670604</v>
       </c>
-      <c r="F43" s="64">
+      <c r="F43" s="43">
         <f t="shared" si="4"/>
         <v>43920.471772593621</v>
       </c>
-      <c r="G43" s="64">
+      <c r="G43" s="43">
         <f t="shared" si="5"/>
         <v>65360.330018139255</v>
       </c>
-      <c r="H43" s="65">
+      <c r="H43" s="44">
         <f t="shared" si="6"/>
         <v>12675.469804818415</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="K32:M32"/>
     <mergeCell ref="K33:M33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Kerosene Decline and tidy #Retrofit Control
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_Retrofit-Ctrl.xlsx
+++ b/SuppXLS/Scen_B_RSD_Retrofit-Ctrl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8EEA61-FD2E-4857-B23E-F9476E806EB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9315D5EB-74B5-4F3B-A56D-52C0DEA0910A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="136">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -594,7 +594,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -739,8 +739,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -807,8 +814,14 @@
         <bgColor theme="7" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1166,19 +1179,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1348,12 +1348,6 @@
     <xf numFmtId="3" fontId="1" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1363,6 +1357,24 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1399,23 +1411,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="21" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2552,12 +2552,12 @@
       <c r="Z15" s="15"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="18"/>
@@ -2641,11 +2641,11 @@
       <c r="A19" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -2673,11 +2673,11 @@
       <c r="A20" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
       <c r="G20" s="24"/>
@@ -2765,11 +2765,11 @@
       <c r="A23" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
@@ -2795,11 +2795,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -2855,11 +2855,11 @@
       <c r="A26" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
@@ -2885,11 +2885,11 @@
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -2977,11 +2977,11 @@
       <c r="A30" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
       <c r="G30" s="15"/>
@@ -3009,11 +3009,11 @@
       <c r="A31" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="60" t="s">
+      <c r="B31" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
       <c r="G31" s="15"/>
@@ -5737,10 +5737,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5838,15 +5838,15 @@
         <v>1</v>
       </c>
       <c r="F8" s="51">
-        <f>($E$72*F$29)/1000</f>
+        <f>($E$54*F$29)/1000</f>
         <v>3.042234442534121</v>
       </c>
       <c r="G8" s="51">
-        <f>(E72*G$28)/1000</f>
+        <f>(E54*G$28)/1000</f>
         <v>11.408379159502955</v>
       </c>
       <c r="H8" s="51">
-        <f>(H72*H$27)/1000</f>
+        <f>(H54*H$27)/1000</f>
         <v>12.041696314577493</v>
       </c>
       <c r="I8" s="2">
@@ -5875,15 +5875,15 @@
         <v>1</v>
       </c>
       <c r="F9" s="51">
-        <f>($E$71*F$29)/1000</f>
+        <f>($E$53*F$29)/1000</f>
         <v>2.4662346453768067</v>
       </c>
       <c r="G9" s="51">
-        <f>(E71*G$28)/1000</f>
+        <f>(E53*G$28)/1000</f>
         <v>9.2483799201630248</v>
       </c>
       <c r="H9" s="51">
-        <f>(H71*H$27)/1000</f>
+        <f>(H53*H$27)/1000</f>
         <v>9.7617883174643403</v>
       </c>
       <c r="I9" s="2">
@@ -5912,15 +5912,15 @@
         <v>1</v>
       </c>
       <c r="F10" s="51">
-        <f>($E$70*F$29)/1000</f>
+        <f>($E$52*F$29)/1000</f>
         <v>5.153575294552267</v>
       </c>
       <c r="G10" s="51">
-        <f>(E70*G$28)/1000</f>
+        <f>(E52*G$28)/1000</f>
         <v>19.325907354571001</v>
       </c>
       <c r="H10" s="51">
-        <f>(H70*H$27)/1000</f>
+        <f>(H52*H$27)/1000</f>
         <v>20.398752891514416</v>
       </c>
       <c r="I10" s="2">
@@ -5949,15 +5949,15 @@
         <v>1</v>
       </c>
       <c r="F11" s="51">
-        <f>($E$69*F$29)/1000</f>
+        <f>($E$51*F$29)/1000</f>
         <v>8.7478683298212321</v>
       </c>
       <c r="G11" s="51">
-        <f>(E69*G$28)/1000</f>
+        <f>(E51*G$28)/1000</f>
         <v>32.804506236829617</v>
       </c>
       <c r="H11" s="51">
-        <f>(H69*H$27)/1000</f>
+        <f>(H51*H$27)/1000</f>
         <v>34.62559372639015</v>
       </c>
       <c r="I11" s="2">
@@ -5986,15 +5986,15 @@
         <v>1</v>
       </c>
       <c r="F12" s="51">
-        <f>($E$68*F$29)/1000</f>
+        <f>($E$50*F$29)/1000</f>
         <v>11.78096068728674</v>
       </c>
       <c r="G12" s="51">
-        <f>(E68*G$28)/1000</f>
+        <f>(E50*G$28)/1000</f>
         <v>44.178602577325279</v>
       </c>
       <c r="H12" s="51">
-        <f>(H68*H$27)/1000</f>
+        <f>(H50*H$27)/1000</f>
         <v>46.6311040684012</v>
       </c>
       <c r="I12" s="2">
@@ -6023,15 +6023,15 @@
         <v>1</v>
       </c>
       <c r="F13" s="52">
-        <f>($E$67*F$29)/1000</f>
+        <f>($E$49*F$29)/1000</f>
         <v>3.9848960750111653</v>
       </c>
       <c r="G13" s="52">
-        <f>(E67*G$28)/1000</f>
+        <f>(E49*G$28)/1000</f>
         <v>14.943360281291868</v>
       </c>
       <c r="H13" s="52">
-        <f>(H67*H$27)/1000</f>
+        <f>(H49*H$27)/1000</f>
         <v>15.772916021707317</v>
       </c>
       <c r="I13" s="49">
@@ -6060,15 +6060,15 @@
         <v>1</v>
       </c>
       <c r="F14" s="53">
-        <f>($C$72*F$29)/1000</f>
+        <f>($C$54*F$29)/1000</f>
         <v>10.541334878817622</v>
       </c>
       <c r="G14" s="53">
-        <f>(C72*G$28)/1000</f>
+        <f>(C54*G$28)/1000</f>
         <v>39.530005795566083</v>
       </c>
       <c r="H14" s="53">
-        <f>(F72*H$27)/1000</f>
+        <f>(F54*H$27)/1000</f>
         <v>41.724448183963943</v>
       </c>
       <c r="I14" s="50">
@@ -6097,15 +6097,15 @@
         <v>1</v>
       </c>
       <c r="F15" s="54">
-        <f>($C$71*F$29)/1000</f>
+        <f>($C$53*F$29)/1000</f>
         <v>10.024761205464234</v>
       </c>
       <c r="G15" s="54">
-        <f>(C71*G$28)/1000</f>
+        <f>(C53*G$28)/1000</f>
         <v>37.592854520490874</v>
       </c>
       <c r="H15" s="54">
-        <f>(F71*H$27)/1000</f>
+        <f>(F53*H$27)/1000</f>
         <v>39.679759184438389</v>
       </c>
       <c r="I15" s="13">
@@ -6134,15 +6134,15 @@
         <v>1</v>
       </c>
       <c r="F16" s="54">
-        <f>($C$70*F$29)/1000</f>
+        <f>($C$52*F$29)/1000</f>
         <v>20.283779192369344</v>
       </c>
       <c r="G16" s="54">
-        <f>(C70*G$28)/1000</f>
+        <f>(C52*G$28)/1000</f>
         <v>76.064171971385051</v>
       </c>
       <c r="H16" s="54">
-        <f>(F70*H$27)/1000</f>
+        <f>(F52*H$27)/1000</f>
         <v>80.286747704756522</v>
       </c>
       <c r="I16" s="13">
@@ -6171,15 +6171,15 @@
         <v>1</v>
       </c>
       <c r="F17" s="54">
-        <f>($C$69*F$29)/1000</f>
+        <f>($C$51*F$29)/1000</f>
         <v>37.525404475322098</v>
       </c>
       <c r="G17" s="54">
-        <f>(C69*G$28)/1000</f>
+        <f>(C51*G$28)/1000</f>
         <v>140.72026678245786</v>
       </c>
       <c r="H17" s="54">
-        <f>(F69*H$27)/1000</f>
+        <f>(F51*H$27)/1000</f>
         <v>148.53211785910801</v>
       </c>
       <c r="I17" s="13">
@@ -6208,15 +6208,15 @@
         <v>1</v>
       </c>
       <c r="F18" s="54">
-        <f>($C$68*F$29)/1000</f>
+        <f>($C$50*F$29)/1000</f>
         <v>56.430305495129602</v>
       </c>
       <c r="G18" s="54">
-        <f>(C68*G$28)/1000</f>
+        <f>(C50*G$28)/1000</f>
         <v>211.61364560673599</v>
       </c>
       <c r="H18" s="54">
-        <f>(F68*H$27)/1000</f>
+        <f>(F50*H$27)/1000</f>
         <v>223.3610244531846</v>
       </c>
       <c r="I18" s="13">
@@ -6245,15 +6245,15 @@
         <v>1</v>
       </c>
       <c r="F19" s="52">
-        <f>($C$67*F$29)/1000</f>
+        <f>($C$49*F$29)/1000</f>
         <v>9.9537699371858963</v>
       </c>
       <c r="G19" s="52">
-        <f>(C67*G$28)/1000</f>
+        <f>(C49*G$28)/1000</f>
         <v>37.326637264447108</v>
       </c>
       <c r="H19" s="52">
-        <f>(F67*H$27)/1000</f>
+        <f>(F49*H$27)/1000</f>
         <v>39.398763321120782</v>
       </c>
       <c r="I19" s="49">
@@ -6282,15 +6282,15 @@
         <v>1</v>
       </c>
       <c r="F20" s="53">
-        <f>($D$72*F$29)/1000</f>
+        <f>($D$54*F$29)/1000</f>
         <v>15.687106688620966</v>
       </c>
       <c r="G20" s="53">
-        <f>(D72*G$28)/1000</f>
+        <f>(D54*G$28)/1000</f>
         <v>58.826650082328619</v>
       </c>
       <c r="H20" s="53">
-        <f>(G72*H$27)/1000</f>
+        <f>(G54*H$27)/1000</f>
         <v>62.092313517232284</v>
       </c>
       <c r="I20" s="50">
@@ -6319,15 +6319,15 @@
         <v>1</v>
       </c>
       <c r="F21" s="54">
-        <f>($D$71*F$29)/1000</f>
+        <f>($D$53*F$29)/1000</f>
         <v>8.6482011525934226</v>
       </c>
       <c r="G21" s="54">
-        <f>(D71*G$28)/1000</f>
+        <f>(D53*G$28)/1000</f>
         <v>32.43075432222534</v>
       </c>
       <c r="H21" s="54">
-        <f>(G71*H$27)/1000</f>
+        <f>(G53*H$27)/1000</f>
         <v>34.23109359716647</v>
       </c>
       <c r="I21" s="13">
@@ -6356,15 +6356,15 @@
         <v>1</v>
       </c>
       <c r="F22" s="54">
-        <f>($D$70*F$29)/1000</f>
+        <f>($D$52*F$29)/1000</f>
         <v>16.279339597911104</v>
       </c>
       <c r="G22" s="54">
-        <f>(D70*G$28)/1000</f>
+        <f>(D52*G$28)/1000</f>
         <v>61.047523492166633</v>
       </c>
       <c r="H22" s="54">
-        <f>(G70*H$27)/1000</f>
+        <f>(G52*H$27)/1000</f>
         <v>64.436475012961779</v>
       </c>
       <c r="I22" s="13">
@@ -6393,15 +6393,15 @@
         <v>1</v>
       </c>
       <c r="F23" s="54">
-        <f>($D$69*F$29)/1000</f>
+        <f>($D$51*F$29)/1000</f>
         <v>33.333558282558243</v>
       </c>
       <c r="G23" s="54">
-        <f>(D69*G$28)/1000</f>
+        <f>(D51*G$28)/1000</f>
         <v>125.00084355959343</v>
       </c>
       <c r="H23" s="54">
-        <f>(G69*H$27)/1000</f>
+        <f>(G51*H$27)/1000</f>
         <v>131.94005705506501</v>
       </c>
       <c r="I23" s="13">
@@ -6430,15 +6430,15 @@
         <v>1</v>
       </c>
       <c r="F24" s="54">
-        <f>($D$68*F$29)/1000</f>
+        <f>($D$50*F$29)/1000</f>
         <v>50.263786722748698</v>
       </c>
       <c r="G24" s="54">
-        <f>(D68*G$28)/1000</f>
+        <f>(D50*G$28)/1000</f>
         <v>188.48920021030762</v>
       </c>
       <c r="H24" s="54">
-        <f>(G68*H$27)/1000</f>
+        <f>(G50*H$27)/1000</f>
         <v>198.9528640113158</v>
       </c>
       <c r="I24" s="13">
@@ -6467,15 +6467,15 @@
         <v>1</v>
       </c>
       <c r="F25" s="52">
-        <f>($D$67*F$29)/1000</f>
+        <f>($D$49*F$29)/1000</f>
         <v>10.693242008796334</v>
       </c>
       <c r="G25" s="52">
-        <f>(D67*G$28)/1000</f>
+        <f>(D49*G$28)/1000</f>
         <v>40.099657532986257</v>
       </c>
       <c r="H25" s="52">
-        <f>(G67*H$27)/1000</f>
+        <f>(G49*H$27)/1000</f>
         <v>42.32572318816743</v>
       </c>
       <c r="I25" s="49">
@@ -6488,47 +6488,47 @@
     </row>
     <row r="26" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="67" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="65"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="69"/>
       <c r="G27" s="2"/>
       <c r="H27" s="30">
         <v>0.95</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="67"/>
-      <c r="E28" s="68"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="72"/>
       <c r="G28" s="30">
         <v>0.75</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="69" t="s">
+      <c r="C29" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="71"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="75"/>
       <c r="F29" s="31">
         <v>0.2</v>
       </c>
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F30" s="59">
+      <c r="F30" s="79">
         <f>SUM(F8:F25)</f>
         <v>314.84035911209992</v>
       </c>
-      <c r="G30" s="59">
+      <c r="G30" s="79">
         <f>SUM(G8:G25)</f>
         <v>1180.6513466703743</v>
       </c>
-      <c r="H30" s="59">
+      <c r="H30" s="79">
         <f>SUM(H8:H25)</f>
         <v>1246.1932384285358</v>
       </c>
@@ -6539,7 +6539,7 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
         <v>1</v>
       </c>
@@ -6567,11 +6567,8 @@
       <c r="I33" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str">
         <f>"UC_RSD_RTFT_Apt"</f>
         <v>UC_RSD_RTFT_Apt</v>
@@ -6590,25 +6587,22 @@
         <v>1</v>
       </c>
       <c r="F34" s="51">
-        <f>(SUM($E$67:$E$72)*F$58)/1000</f>
+        <f>(SUM($E$49:$E$54)*F$40)/1000</f>
         <v>0</v>
       </c>
       <c r="G34" s="51">
-        <f>(SUM($E$67:$E$72)*G$57)/1000</f>
+        <f>(SUM($E$49:$E$54)*G$39)/1000</f>
         <v>17.587884737291166</v>
       </c>
       <c r="H34" s="51">
-        <f>(SUM($H$67:$H$72)*H$56)/1000</f>
+        <f>(SUM($H$49:$H$54)*H$38)/1000</f>
         <v>36.639960878961823</v>
       </c>
       <c r="I34" s="2">
         <v>5</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="str">
         <f>"UC_RSD_RTFT_Att"</f>
         <v>UC_RSD_RTFT_Att</v>
@@ -6627,22 +6621,22 @@
         <v>1</v>
       </c>
       <c r="F35" s="51">
-        <f>(SUM($C$67:$C$72)*F$58)/1000</f>
+        <f>(SUM($C$49:$C$54)*F$40)/1000</f>
         <v>0</v>
       </c>
       <c r="G35" s="51">
-        <f>(SUM($C$67:$C$72)*G$57)/1000</f>
+        <f>(SUM($C$49:$C$54)*G$39)/1000</f>
         <v>72.37967759214439</v>
       </c>
       <c r="H35" s="51">
-        <f>(SUM($F$67:$F$72)*H$56)/1000</f>
+        <f>(SUM($F$49:$F$54)*H$38)/1000</f>
         <v>150.78496334383479</v>
       </c>
       <c r="I35" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="str">
         <f>"UC_RSD_RTFT_Det"</f>
         <v>UC_RSD_RTFT_Det</v>
@@ -6661,1010 +6655,379 @@
         <v>1</v>
       </c>
       <c r="F36" s="51">
-        <f>(SUM($D$67:$D$72)*F$58)/1000</f>
+        <f>(SUM($D$49:$D$54)*F$40)/1000</f>
         <v>0</v>
       </c>
       <c r="G36" s="51">
-        <f>(SUM($D$67:$D$72)*G$57)/1000</f>
+        <f>(SUM($D$49:$D$54)*G$39)/1000</f>
         <v>67.452617226614393</v>
       </c>
       <c r="H36" s="51">
-        <f>(SUM($G$67:$G$72)*H$56)/1000</f>
+        <f>(SUM($G$49:$G$54)*H$38)/1000</f>
         <v>140.52066483734444</v>
       </c>
       <c r="I36" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F37" s="51"/>
       <c r="G37" s="51"/>
       <c r="H37" s="51"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="str">
-        <f t="shared" ref="A38:A41" si="4">"UC_RSD_RTFT_"&amp;RIGHT(C38,5)</f>
-        <v>UC_RSD_RTFT_Apt_F</v>
-      </c>
-      <c r="B38" s="2" t="str">
-        <f t="shared" ref="B38:B41" si="5">"Maximum number of deep retrofits from Apartment_" &amp;RIGHT(C38,1)</f>
-        <v>Maximum number of deep retrofits from Apartment_F</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1</v>
-      </c>
-      <c r="F38" s="51">
-        <f>($E$71*F$58)/1000</f>
+    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" s="68"/>
+      <c r="E38" s="69"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="30">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="70" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="71"/>
+      <c r="E39" s="72"/>
+      <c r="G39" s="30">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="74"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="31">
         <v>0</v>
       </c>
-      <c r="G38" s="51">
-        <f>(E71*G$57)/1000</f>
-        <v>1.2331173226884034</v>
-      </c>
-      <c r="H38" s="51">
-        <f>(H71*H$56)/1000</f>
-        <v>2.5688916624906164</v>
-      </c>
-      <c r="I38" s="2">
-        <v>5</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="str">
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F41" s="79">
+        <f>SUM(F34:F37)</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="79">
+        <f>SUM(G34:G36)</f>
+        <v>157.42017955604996</v>
+      </c>
+      <c r="H41" s="79">
+        <f>SUM(H34:H37)</f>
+        <v>327.94558906014106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="76" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="77"/>
+      <c r="D43" s="77"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="78"/>
+      <c r="K43" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="L43" s="62"/>
+      <c r="M43" s="63"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="32"/>
+      <c r="C44" s="76">
+        <v>2018</v>
+      </c>
+      <c r="D44" s="77"/>
+      <c r="E44" s="78"/>
+      <c r="F44" s="67">
+        <v>2070</v>
+      </c>
+      <c r="G44" s="68"/>
+      <c r="H44" s="69"/>
+      <c r="K44" s="64">
+        <v>0.83330000000000004</v>
+      </c>
+      <c r="L44" s="65"/>
+      <c r="M44" s="66"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="G45" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="H45" s="47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="B46" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="55">
+        <v>37224.073727176743</v>
+      </c>
+      <c r="D46" s="55">
+        <v>31387.706337556119</v>
+      </c>
+      <c r="E46" s="55">
+        <v>14540.898856806734</v>
+      </c>
+      <c r="F46" s="34">
+        <f>C46*$K$44</f>
+        <v>31018.820636856381</v>
+      </c>
+      <c r="G46" s="34">
+        <f>D46*$K$44</f>
+        <v>26155.375691085515</v>
+      </c>
+      <c r="H46" s="39">
+        <f>E46*$K$44</f>
+        <v>12116.931017377052</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="B47" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" s="56">
+        <v>9537.7783975583752</v>
+      </c>
+      <c r="D47" s="56">
+        <v>9433.9012004747347</v>
+      </c>
+      <c r="E47" s="56">
+        <v>7459.2913438514906</v>
+      </c>
+      <c r="F47" s="36">
+        <f t="shared" ref="F47:F54" si="4">C47*$K$44</f>
+        <v>7947.8307386853949</v>
+      </c>
+      <c r="G47" s="36">
+        <f t="shared" ref="G47:G54" si="5">D47*$K$44</f>
+        <v>7861.269870355597</v>
+      </c>
+      <c r="H47" s="40">
+        <f t="shared" ref="H47:H54" si="6">E47*$K$44</f>
+        <v>6215.8274768314477</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="B48" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="57">
+        <v>17545.09295382088</v>
+      </c>
+      <c r="D48" s="57">
+        <v>20090.949195825138</v>
+      </c>
+      <c r="E48" s="57">
+        <v>14041.847426430093</v>
+      </c>
+      <c r="F48" s="38">
         <f t="shared" si="4"/>
-        <v>UC_RSD_RTFT_Apt_E</v>
-      </c>
-      <c r="B39" s="2" t="str">
+        <v>14620.32595841894</v>
+      </c>
+      <c r="G48" s="38">
         <f t="shared" si="5"/>
-        <v>Maximum number of deep retrofits from Apartment_E</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" s="2">
-        <v>1</v>
-      </c>
-      <c r="F39" s="51">
-        <f>($E$70*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G39" s="51">
-        <f>(E70*G$57)/1000</f>
-        <v>2.5767876472761335</v>
-      </c>
-      <c r="H39" s="51">
-        <f>(H70*H$56)/1000</f>
-        <v>5.3680928661880056</v>
-      </c>
-      <c r="I39" s="2">
-        <v>5</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="str">
+        <v>16741.787964881089</v>
+      </c>
+      <c r="H48" s="41">
+        <f t="shared" si="6"/>
+        <v>11701.071460444196</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B49" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="56">
+        <v>49768.849685929476</v>
+      </c>
+      <c r="D49" s="56">
+        <v>53466.210043981671</v>
+      </c>
+      <c r="E49" s="56">
+        <v>19924.480375055824</v>
+      </c>
+      <c r="F49" s="36">
         <f t="shared" si="4"/>
-        <v>UC_RSD_RTFT_Apt_D</v>
-      </c>
-      <c r="B40" s="2" t="str">
+        <v>41472.382443285031</v>
+      </c>
+      <c r="G49" s="36">
         <f t="shared" si="5"/>
-        <v>Maximum number of deep retrofits from Apartment_D</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="2">
-        <v>1</v>
-      </c>
-      <c r="F40" s="51">
-        <f>($E$69*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="51">
-        <f>(E69*G$57)/1000</f>
-        <v>4.373934164910616</v>
-      </c>
-      <c r="H40" s="51">
-        <f>(H69*H$56)/1000</f>
-        <v>9.1119983490500402</v>
-      </c>
-      <c r="I40" s="2">
-        <v>5</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="str">
+        <v>44553.392829649929</v>
+      </c>
+      <c r="H49" s="40">
+        <f t="shared" si="6"/>
+        <v>16603.069496534019</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B50" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" s="57">
+        <v>282151.52747564798</v>
+      </c>
+      <c r="D50" s="57">
+        <v>251318.93361374349</v>
+      </c>
+      <c r="E50" s="57">
+        <v>58904.8034364337</v>
+      </c>
+      <c r="F50" s="38">
         <f t="shared" si="4"/>
-        <v>UC_RSD_RTFT_Apt_C</v>
-      </c>
-      <c r="B41" s="2" t="str">
+        <v>235116.86784545748</v>
+      </c>
+      <c r="G50" s="38">
         <f t="shared" si="5"/>
-        <v>Maximum number of deep retrofits from Apartment_C</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E41" s="2">
-        <v>1</v>
-      </c>
-      <c r="F41" s="51">
-        <f>($E$68*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G41" s="51">
-        <f>(E68*G$57)/1000</f>
-        <v>5.8904803436433699</v>
-      </c>
-      <c r="H41" s="51">
-        <f>(H68*H$56)/1000</f>
-        <v>12.271343175895051</v>
-      </c>
-      <c r="I41" s="2">
-        <v>5</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="str">
-        <f>"UC_RSD_RTFT_"&amp;RIGHT(C42,6)</f>
-        <v>UC_RSD_RTFT_Apt_B3</v>
-      </c>
-      <c r="B42" s="49" t="str">
-        <f>"Maximum number of deep retrofits from Apartment_" &amp;RIGHT(C42,2)</f>
-        <v>Maximum number of deep retrofits from Apartment_B3</v>
-      </c>
-      <c r="C42" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" s="49" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="49">
-        <v>1</v>
-      </c>
-      <c r="F42" s="52">
-        <f>($E$67*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G42" s="52">
-        <f>(E67*G$57)/1000</f>
-        <v>1.9924480375055826</v>
-      </c>
-      <c r="H42" s="52">
-        <f>(H67*H$56)/1000</f>
-        <v>4.1507673741335047</v>
-      </c>
-      <c r="I42" s="49">
-        <v>5</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="50" t="str">
-        <f>"UC_RSD_RTFT_"&amp;RIGHT(C43,5)</f>
-        <v>UC_RSD_RTFT_Att_G</v>
-      </c>
-      <c r="B43" s="50" t="str">
-        <f>"Maximum number of deep retrofits from Attached_" &amp;RIGHT(C43,1)</f>
-        <v>Maximum number of deep retrofits from Attached_G</v>
-      </c>
-      <c r="C43" s="50" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="50">
-        <v>1</v>
-      </c>
-      <c r="F43" s="53">
-        <f>($C$72*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G43" s="53">
-        <f>(C72*G$57)/1000</f>
-        <v>5.2706674394088111</v>
-      </c>
-      <c r="H43" s="53">
-        <f>(F72*H$56)/1000</f>
-        <v>10.980117943148406</v>
-      </c>
-      <c r="I43" s="50">
-        <v>5</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="str">
-        <f t="shared" ref="A44:A47" si="6">"UC_RSD_RTFT_"&amp;RIGHT(C44,5)</f>
-        <v>UC_RSD_RTFT_Att_F</v>
-      </c>
-      <c r="B44" s="13" t="str">
-        <f>"Maximum number of deep retrofits from Attached_" &amp;RIGHT(C44,1)</f>
-        <v>Maximum number of deep retrofits from Attached_F</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="13">
-        <v>1</v>
-      </c>
-      <c r="F44" s="54">
-        <f>($C$71*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G44" s="54">
-        <f>(C71*G$57)/1000</f>
-        <v>5.0123806027321169</v>
-      </c>
-      <c r="H44" s="54">
-        <f>(F71*H$56)/1000</f>
-        <v>10.442041890641681</v>
-      </c>
-      <c r="I44" s="13">
-        <v>5</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="str">
+        <v>209424.06738033245</v>
+      </c>
+      <c r="H50" s="41">
         <f t="shared" si="6"/>
-        <v>UC_RSD_RTFT_Att_E</v>
-      </c>
-      <c r="B45" s="13" t="str">
-        <f>"Maximum number of deep retrofits from Attached_" &amp;RIGHT(C45,1)</f>
-        <v>Maximum number of deep retrofits from Attached_E</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E45" s="13">
-        <v>1</v>
-      </c>
-      <c r="F45" s="54">
-        <f>($C$70*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G45" s="54">
-        <f>(C70*G$57)/1000</f>
-        <v>10.141889596184672</v>
-      </c>
-      <c r="H45" s="54">
-        <f>(F70*H$56)/1000</f>
-        <v>21.128091501251717</v>
-      </c>
-      <c r="I45" s="13">
-        <v>5</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="13" t="str">
+        <v>49085.372703580208</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B51" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" s="56">
+        <v>187627.02237661046</v>
+      </c>
+      <c r="D51" s="56">
+        <v>166667.79141279124</v>
+      </c>
+      <c r="E51" s="56">
+        <v>43739.341649106158</v>
+      </c>
+      <c r="F51" s="36">
+        <f t="shared" si="4"/>
+        <v>156349.5977464295</v>
+      </c>
+      <c r="G51" s="36">
+        <f t="shared" si="5"/>
+        <v>138884.27058427894</v>
+      </c>
+      <c r="H51" s="40">
         <f t="shared" si="6"/>
-        <v>UC_RSD_RTFT_Att_D</v>
-      </c>
-      <c r="B46" s="13" t="str">
-        <f>"Maximum number of deep retrofits from Attached_" &amp;RIGHT(C46,1)</f>
-        <v>Maximum number of deep retrofits from Attached_D</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E46" s="13">
-        <v>1</v>
-      </c>
-      <c r="F46" s="54">
-        <f>($C$69*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="54">
-        <f>(C69*G$57)/1000</f>
-        <v>18.762702237661049</v>
-      </c>
-      <c r="H46" s="54">
-        <f>(F69*H$56)/1000</f>
-        <v>39.087399436607377</v>
-      </c>
-      <c r="I46" s="13">
-        <v>5</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="str">
+        <v>36447.99339620016</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B52" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" s="57">
+        <v>101418.89596184672</v>
+      </c>
+      <c r="D52" s="57">
+        <v>81396.697989555512</v>
+      </c>
+      <c r="E52" s="57">
+        <v>25767.876472761334</v>
+      </c>
+      <c r="F52" s="38">
+        <f t="shared" si="4"/>
+        <v>84512.366005006872</v>
+      </c>
+      <c r="G52" s="38">
+        <f t="shared" si="5"/>
+        <v>67827.868434696618</v>
+      </c>
+      <c r="H52" s="41">
         <f t="shared" si="6"/>
-        <v>UC_RSD_RTFT_Att_C</v>
-      </c>
-      <c r="B47" s="13" t="str">
-        <f>"Maximum number of deep retrofits from Attached_" &amp;RIGHT(C47,1)</f>
-        <v>Maximum number of deep retrofits from Attached_C</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E47" s="13">
-        <v>1</v>
-      </c>
-      <c r="F47" s="54">
-        <f>($C$68*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G47" s="54">
-        <f>(C68*G$57)/1000</f>
-        <v>28.215152747564801</v>
-      </c>
-      <c r="H47" s="54">
-        <f>(F68*H$56)/1000</f>
-        <v>58.779216961364369</v>
-      </c>
-      <c r="I47" s="13">
-        <v>5</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="49" t="str">
-        <f>"UC_RSD_RTFT_"&amp;RIGHT(C48,6)</f>
-        <v>UC_RSD_RTFT_Att_B3</v>
-      </c>
-      <c r="B48" s="49" t="str">
-        <f>"Maximum number of deep retrofits from Attached_" &amp;RIGHT(C48,2)</f>
-        <v>Maximum number of deep retrofits from Attached_B3</v>
-      </c>
-      <c r="C48" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="D48" s="49" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" s="49">
-        <v>1</v>
-      </c>
-      <c r="F48" s="52">
-        <f>($C$67*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G48" s="52">
-        <f>(C67*G$57)/1000</f>
-        <v>4.9768849685929482</v>
-      </c>
-      <c r="H48" s="52">
-        <f>(F67*H$56)/1000</f>
-        <v>10.368095610821257</v>
-      </c>
-      <c r="I48" s="49">
-        <v>5</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="50" t="str">
-        <f>"UC_RSD_RTFT_"&amp;RIGHT(C49,5)</f>
-        <v>UC_RSD_RTFT_Det_G</v>
-      </c>
-      <c r="B49" s="50" t="str">
-        <f>"Maximum number of deep retrofits from Detached_" &amp;RIGHT(C49,1)</f>
-        <v>Maximum number of deep retrofits from Detached_G</v>
-      </c>
-      <c r="C49" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E49" s="50">
-        <v>1</v>
-      </c>
-      <c r="F49" s="53">
-        <f>($D$72*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="53">
-        <f>(D72*G$57)/1000</f>
-        <v>7.8435533443104832</v>
-      </c>
-      <c r="H49" s="53">
-        <f>(G72*H$56)/1000</f>
-        <v>16.340082504534813</v>
-      </c>
-      <c r="I49" s="50">
-        <v>5</v>
-      </c>
-      <c r="K49" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="str">
-        <f t="shared" ref="A50:A53" si="7">"UC_RSD_RTFT_"&amp;RIGHT(C50,5)</f>
-        <v>UC_RSD_RTFT_Det_F</v>
-      </c>
-      <c r="B50" s="13" t="str">
-        <f>"Maximum number of deep retrofits from Detached_" &amp;RIGHT(C50,1)</f>
-        <v>Maximum number of deep retrofits from Detached_F</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E50" s="13">
-        <v>1</v>
-      </c>
-      <c r="F50" s="54">
-        <f>($D$71*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="54">
-        <f>(D71*G$57)/1000</f>
-        <v>4.3241005762967113</v>
-      </c>
-      <c r="H50" s="54">
-        <f>(G71*H$56)/1000</f>
-        <v>9.008182525570124</v>
-      </c>
-      <c r="I50" s="13">
-        <v>5</v>
-      </c>
-      <c r="K50" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="13" t="str">
-        <f t="shared" si="7"/>
-        <v>UC_RSD_RTFT_Det_E</v>
-      </c>
-      <c r="B51" s="13" t="str">
-        <f>"Maximum number of deep retrofits from Detached_" &amp;RIGHT(C51,1)</f>
-        <v>Maximum number of deep retrofits from Detached_E</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E51" s="13">
-        <v>1</v>
-      </c>
-      <c r="F51" s="54">
-        <f>($D$70*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G51" s="54">
-        <f>(D70*G$57)/1000</f>
-        <v>8.139669798955552</v>
-      </c>
-      <c r="H51" s="54">
-        <f>(G70*H$56)/1000</f>
-        <v>16.956967108674153</v>
-      </c>
-      <c r="I51" s="13">
-        <v>5</v>
-      </c>
-      <c r="K51" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="str">
-        <f t="shared" si="7"/>
-        <v>UC_RSD_RTFT_Det_D</v>
-      </c>
-      <c r="B52" s="13" t="str">
-        <f>"Maximum number of deep retrofits from Detached_" &amp;RIGHT(C52,1)</f>
-        <v>Maximum number of deep retrofits from Detached_D</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E52" s="13">
-        <v>1</v>
-      </c>
-      <c r="F52" s="54">
-        <f>($D$69*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G52" s="54">
-        <f>(D69*G$57)/1000</f>
-        <v>16.666779141279122</v>
-      </c>
-      <c r="H52" s="54">
-        <f>(G69*H$56)/1000</f>
-        <v>34.721067646069734</v>
-      </c>
-      <c r="I52" s="13">
-        <v>5</v>
-      </c>
-      <c r="K52" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A53" s="13" t="str">
-        <f t="shared" si="7"/>
-        <v>UC_RSD_RTFT_Det_C</v>
-      </c>
-      <c r="B53" s="13" t="str">
-        <f>"Maximum number of deep retrofits from Detached_" &amp;RIGHT(C53,1)</f>
-        <v>Maximum number of deep retrofits from Detached_C</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E53" s="13">
-        <v>1</v>
-      </c>
-      <c r="F53" s="54">
-        <f>($D$68*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G53" s="54">
-        <f>(D68*G$57)/1000</f>
-        <v>25.131893361374349</v>
-      </c>
-      <c r="H53" s="54">
-        <f>(G68*H$56)/1000</f>
-        <v>52.356016845083111</v>
-      </c>
-      <c r="I53" s="13">
-        <v>5</v>
-      </c>
-      <c r="K53" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="49" t="str">
-        <f>"UC_RSD_RTFT_"&amp;RIGHT(C54,6)</f>
-        <v>UC_RSD_RTFT_Det_B3</v>
-      </c>
-      <c r="B54" s="49" t="str">
-        <f>"Maximum number of deep retrofits from Detached_" &amp;RIGHT(C54,2)</f>
-        <v>Maximum number of deep retrofits from Detached_B3</v>
-      </c>
-      <c r="C54" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="D54" s="49" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" s="49">
-        <v>1</v>
-      </c>
-      <c r="F54" s="52">
-        <f>($D$67*F$58)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="G54" s="52">
-        <f>(D67*G$57)/1000</f>
-        <v>5.346621004398167</v>
-      </c>
-      <c r="H54" s="52">
-        <f>(G67*H$56)/1000</f>
-        <v>11.138348207412482</v>
-      </c>
-      <c r="I54" s="49">
-        <v>5</v>
-      </c>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="63" t="s">
-        <v>130</v>
-      </c>
-      <c r="D56" s="64"/>
-      <c r="E56" s="65"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="30">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="D57" s="67"/>
-      <c r="E57" s="68"/>
-      <c r="G57" s="30">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="69" t="s">
-        <v>132</v>
-      </c>
-      <c r="D58" s="70"/>
-      <c r="E58" s="71"/>
-      <c r="F58" s="31">
-        <v>0</v>
-      </c>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F59" s="59">
-        <f>SUM(F34:F54)</f>
-        <v>0</v>
-      </c>
-      <c r="G59" s="59">
-        <f>SUM(G34:G54)</f>
-        <v>313.31924189083281</v>
-      </c>
-      <c r="H59" s="59">
-        <f>SUM(H34:H54)</f>
-        <v>652.7223106690775</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="72" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" s="73"/>
-      <c r="D61" s="73"/>
-      <c r="E61" s="73"/>
-      <c r="F61" s="73"/>
-      <c r="G61" s="73"/>
-      <c r="H61" s="74"/>
-      <c r="K61" s="75" t="s">
-        <v>113</v>
-      </c>
-      <c r="L61" s="76"/>
-      <c r="M61" s="77"/>
-    </row>
-    <row r="62" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="32"/>
-      <c r="C62" s="72">
-        <v>2018</v>
-      </c>
-      <c r="D62" s="73"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="63">
-        <v>2070</v>
-      </c>
-      <c r="G62" s="64"/>
-      <c r="H62" s="65"/>
-      <c r="K62" s="78">
-        <v>0.83330000000000004</v>
-      </c>
-      <c r="L62" s="79"/>
-      <c r="M62" s="80"/>
-    </row>
-    <row r="63" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="C63" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="D63" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="E63" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="F63" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="G63" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="H63" s="47" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="B64" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C64" s="55">
-        <v>37224.073727176743</v>
-      </c>
-      <c r="D64" s="55">
-        <v>31387.706337556119</v>
-      </c>
-      <c r="E64" s="55">
-        <v>14540.898856806734</v>
-      </c>
-      <c r="F64" s="34">
-        <f>C64*$K$62</f>
-        <v>31018.820636856381</v>
-      </c>
-      <c r="G64" s="34">
-        <f>D64*$K$62</f>
-        <v>26155.375691085515</v>
-      </c>
-      <c r="H64" s="39">
-        <f>E64*$K$62</f>
-        <v>12116.931017377052</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B65" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="C65" s="56">
-        <v>9537.7783975583752</v>
-      </c>
-      <c r="D65" s="56">
-        <v>9433.9012004747347</v>
-      </c>
-      <c r="E65" s="56">
-        <v>7459.2913438514906</v>
-      </c>
-      <c r="F65" s="36">
-        <f t="shared" ref="F65:F72" si="8">C65*$K$62</f>
-        <v>7947.8307386853949</v>
-      </c>
-      <c r="G65" s="36">
-        <f t="shared" ref="G65:G72" si="9">D65*$K$62</f>
-        <v>7861.269870355597</v>
-      </c>
-      <c r="H65" s="40">
-        <f t="shared" ref="H65:H72" si="10">E65*$K$62</f>
-        <v>6215.8274768314477</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B66" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="C66" s="57">
-        <v>17545.09295382088</v>
-      </c>
-      <c r="D66" s="57">
-        <v>20090.949195825138</v>
-      </c>
-      <c r="E66" s="57">
-        <v>14041.847426430093</v>
-      </c>
-      <c r="F66" s="38">
-        <f t="shared" si="8"/>
-        <v>14620.32595841894</v>
-      </c>
-      <c r="G66" s="38">
-        <f t="shared" si="9"/>
-        <v>16741.787964881089</v>
-      </c>
-      <c r="H66" s="41">
-        <f t="shared" si="10"/>
-        <v>11701.071460444196</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B67" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="C67" s="56">
-        <v>49768.849685929476</v>
-      </c>
-      <c r="D67" s="56">
-        <v>53466.210043981671</v>
-      </c>
-      <c r="E67" s="56">
-        <v>19924.480375055824</v>
-      </c>
-      <c r="F67" s="36">
-        <f t="shared" si="8"/>
-        <v>41472.382443285031</v>
-      </c>
-      <c r="G67" s="36">
-        <f t="shared" si="9"/>
-        <v>44553.392829649929</v>
-      </c>
-      <c r="H67" s="40">
-        <f t="shared" si="10"/>
-        <v>16603.069496534019</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B68" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C68" s="57">
-        <v>282151.52747564798</v>
-      </c>
-      <c r="D68" s="57">
-        <v>251318.93361374349</v>
-      </c>
-      <c r="E68" s="57">
-        <v>58904.8034364337</v>
-      </c>
-      <c r="F68" s="38">
-        <f t="shared" si="8"/>
-        <v>235116.86784545748</v>
-      </c>
-      <c r="G68" s="38">
-        <f t="shared" si="9"/>
-        <v>209424.06738033245</v>
-      </c>
-      <c r="H68" s="41">
-        <f t="shared" si="10"/>
-        <v>49085.372703580208</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B69" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="C69" s="56">
-        <v>187627.02237661046</v>
-      </c>
-      <c r="D69" s="56">
-        <v>166667.79141279124</v>
-      </c>
-      <c r="E69" s="56">
-        <v>43739.341649106158</v>
-      </c>
-      <c r="F69" s="36">
-        <f t="shared" si="8"/>
-        <v>156349.5977464295</v>
-      </c>
-      <c r="G69" s="36">
-        <f t="shared" si="9"/>
-        <v>138884.27058427894</v>
-      </c>
-      <c r="H69" s="40">
-        <f t="shared" si="10"/>
-        <v>36447.99339620016</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B70" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="C70" s="57">
-        <v>101418.89596184672</v>
-      </c>
-      <c r="D70" s="57">
-        <v>81396.697989555512</v>
-      </c>
-      <c r="E70" s="57">
-        <v>25767.876472761334</v>
-      </c>
-      <c r="F70" s="38">
-        <f t="shared" si="8"/>
-        <v>84512.366005006872</v>
-      </c>
-      <c r="G70" s="38">
-        <f t="shared" si="9"/>
-        <v>67827.868434696618</v>
-      </c>
-      <c r="H70" s="41">
-        <f t="shared" si="10"/>
         <v>21472.371464752021</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B71" s="35" t="s">
+    <row r="53" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B53" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C71" s="56">
+      <c r="C53" s="56">
         <v>50123.806027321167</v>
       </c>
-      <c r="D71" s="56">
+      <c r="D53" s="56">
         <v>43241.005762967114</v>
       </c>
-      <c r="E71" s="56">
+      <c r="E53" s="56">
         <v>12331.173226884033</v>
       </c>
-      <c r="F71" s="36">
-        <f t="shared" si="8"/>
+      <c r="F53" s="36">
+        <f t="shared" si="4"/>
         <v>41768.167562566727</v>
       </c>
-      <c r="G71" s="36">
-        <f t="shared" si="9"/>
+      <c r="G53" s="36">
+        <f t="shared" si="5"/>
         <v>36032.730102280497</v>
       </c>
-      <c r="H71" s="40">
-        <f t="shared" si="10"/>
+      <c r="H53" s="40">
+        <f t="shared" si="6"/>
         <v>10275.566649962466</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="42" t="s">
+    <row r="54" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="C72" s="58">
+      <c r="C54" s="80">
         <v>52706.674394088106</v>
       </c>
-      <c r="D72" s="58">
+      <c r="D54" s="80">
         <v>78435.533443104825</v>
       </c>
-      <c r="E72" s="58">
+      <c r="E54" s="80">
         <v>15211.172212670604</v>
       </c>
-      <c r="F72" s="43">
-        <f t="shared" si="8"/>
+      <c r="F54" s="43">
+        <f t="shared" si="4"/>
         <v>43920.471772593621</v>
       </c>
-      <c r="G72" s="43">
-        <f t="shared" si="9"/>
+      <c r="G54" s="43">
+        <f t="shared" si="5"/>
         <v>65360.330018139255</v>
       </c>
-      <c r="H72" s="44">
-        <f t="shared" si="10"/>
+      <c r="H54" s="44">
+        <f t="shared" si="6"/>
         <v>12675.469804818415</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="K61:M61"/>
-    <mergeCell ref="K62:M62"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Min 10% RTFT same as WP2 Model
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_Retrofit-Ctrl.xlsx
+++ b/SuppXLS/Scen_B_RSD_Retrofit-Ctrl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E919F3F9-61DE-4883-88AA-3DCC4B9CEB2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FE8A9A-6743-4A48-A084-0D9B737A7180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -1363,6 +1363,42 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1380,42 +1416,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5739,8 +5739,8 @@
   </sheetPr>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6488,32 +6488,32 @@
     </row>
     <row r="26" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="69" t="s">
+      <c r="C27" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="71"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="65"/>
       <c r="G27" s="2"/>
       <c r="H27" s="30">
         <v>0.95</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="72" t="s">
+      <c r="C28" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="73"/>
-      <c r="E28" s="74"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="68"/>
       <c r="G28" s="30">
         <v>0.75</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="76"/>
-      <c r="E29" s="77"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="71"/>
       <c r="F29" s="31">
         <v>0.2</v>
       </c>
@@ -6592,11 +6592,11 @@
       </c>
       <c r="G34" s="51">
         <f>(SUM($E$49:$E$54)*G$39)/1000</f>
-        <v>0</v>
+        <v>17.587884737291166</v>
       </c>
       <c r="H34" s="51">
         <f>(SUM($H$49:$H$54)*H$38)/1000</f>
-        <v>0</v>
+        <v>36.639960878961823</v>
       </c>
       <c r="I34" s="2">
         <v>5</v>
@@ -6626,11 +6626,11 @@
       </c>
       <c r="G35" s="51">
         <f>(SUM($C$49:$C$54)*G$39)/1000</f>
-        <v>0</v>
+        <v>72.37967759214439</v>
       </c>
       <c r="H35" s="51">
         <f>(SUM($F$49:$F$54)*H$38)/1000</f>
-        <v>0</v>
+        <v>150.78496334383479</v>
       </c>
       <c r="I35" s="2">
         <v>5</v>
@@ -6660,11 +6660,11 @@
       </c>
       <c r="G36" s="51">
         <f>(SUM($D$49:$D$54)*G$39)/1000</f>
-        <v>0</v>
+        <v>67.452617226614393</v>
       </c>
       <c r="H36" s="51">
         <f>(SUM($G$49:$G$54)*H$38)/1000</f>
-        <v>0</v>
+        <v>140.52066483734444</v>
       </c>
       <c r="I36" s="2">
         <v>5</v>
@@ -6676,32 +6676,32 @@
       <c r="H37" s="51"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="69" t="s">
+      <c r="C38" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="D38" s="70"/>
-      <c r="E38" s="71"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="G38" s="2"/>
       <c r="H38" s="30">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="72" t="s">
+      <c r="C39" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="74"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="68"/>
       <c r="G39" s="30">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="75" t="s">
+      <c r="C40" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="D40" s="76"/>
-      <c r="E40" s="77"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="71"/>
       <c r="F40" s="31">
         <v>0</v>
       </c>
@@ -6714,49 +6714,49 @@
       </c>
       <c r="G41" s="58">
         <f>SUM(G34:G36)</f>
-        <v>0</v>
+        <v>157.42017955604996</v>
       </c>
       <c r="H41" s="58">
         <f>SUM(H34:H37)</f>
-        <v>0</v>
+        <v>327.94558906014106</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="78" t="s">
+      <c r="B43" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="79"/>
-      <c r="D43" s="79"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="80"/>
-      <c r="K43" s="63" t="s">
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="74"/>
+      <c r="K43" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="L43" s="64"/>
-      <c r="M43" s="65"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="77"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
-      <c r="C44" s="78">
+      <c r="C44" s="72">
         <v>2018</v>
       </c>
-      <c r="D44" s="79"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="69">
+      <c r="D44" s="73"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="63">
         <v>2070</v>
       </c>
-      <c r="G44" s="70"/>
-      <c r="H44" s="71"/>
-      <c r="K44" s="66">
+      <c r="G44" s="64"/>
+      <c r="H44" s="65"/>
+      <c r="K44" s="78">
         <v>0.83330000000000004</v>
       </c>
-      <c r="L44" s="67"/>
-      <c r="M44" s="68"/>
+      <c r="L44" s="79"/>
+      <c r="M44" s="80"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="45" t="s">
@@ -7017,17 +7017,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="F44:H44"/>
     <mergeCell ref="B43:H43"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UC_CAP and NO RTFT UCs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_RSD_Retrofit-Ctrl.xlsx
+++ b/SuppXLS/Scen_B_RSD_Retrofit-Ctrl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23162992-FE52-4AD6-AB19-C22763FC0783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F799DDB6-2283-41DB-9E4A-205D128BAF07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2EA072F4-62CE-45F6-8797-FBD7616D2DDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="3" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="136">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -1363,6 +1363,42 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1380,42 +1416,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2113,7 +2113,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
@@ -5739,8 +5739,8 @@
   </sheetPr>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5750,7 +5750,7 @@
     <col min="3" max="6" width="12.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="12" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="2"/>
     <col min="11" max="11" width="20.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="2"/>
@@ -5781,10 +5781,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="D6" s="1" t="s">
-        <v>72</v>
-      </c>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -6488,32 +6485,32 @@
     </row>
     <row r="26" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="69" t="s">
+      <c r="C27" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="71"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="65"/>
       <c r="G27" s="2"/>
       <c r="H27" s="30">
         <v>0.95</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="72" t="s">
+      <c r="C28" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="73"/>
-      <c r="E28" s="74"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="68"/>
       <c r="G28" s="30">
         <v>0.75</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="76"/>
-      <c r="E29" s="77"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="71"/>
       <c r="F29" s="31">
         <v>0.2</v>
       </c>
@@ -6533,10 +6530,13 @@
         <v>1246.1932384285358</v>
       </c>
     </row>
+    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="D31" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="D32" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="D32" s="1"/>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -6676,32 +6676,32 @@
       <c r="H37" s="51"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="69" t="s">
+      <c r="C38" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="D38" s="70"/>
-      <c r="E38" s="71"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="G38" s="2"/>
       <c r="H38" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="72" t="s">
+      <c r="C39" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="74"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="68"/>
       <c r="G39" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="75" t="s">
+      <c r="C40" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="D40" s="76"/>
-      <c r="E40" s="77"/>
+      <c r="D40" s="70"/>
+      <c r="E40" s="71"/>
       <c r="F40" s="31">
         <v>0</v>
       </c>
@@ -6725,38 +6725,38 @@
       <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="78" t="s">
+      <c r="B43" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="79"/>
-      <c r="D43" s="79"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="80"/>
-      <c r="K43" s="63" t="s">
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="74"/>
+      <c r="K43" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="L43" s="64"/>
-      <c r="M43" s="65"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="77"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
-      <c r="C44" s="78">
+      <c r="C44" s="72">
         <v>2018</v>
       </c>
-      <c r="D44" s="79"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="69">
+      <c r="D44" s="73"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="63">
         <v>2070</v>
       </c>
-      <c r="G44" s="70"/>
-      <c r="H44" s="71"/>
-      <c r="K44" s="66">
+      <c r="G44" s="64"/>
+      <c r="H44" s="65"/>
+      <c r="K44" s="78">
         <v>0.83330000000000004</v>
       </c>
-      <c r="L44" s="67"/>
-      <c r="M44" s="68"/>
+      <c r="L44" s="79"/>
+      <c r="M44" s="80"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="45" t="s">
@@ -7017,17 +7017,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="F44:H44"/>
     <mergeCell ref="B43:H43"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>